<commit_message>
UP Descriptivos análisis correlacional padres->hijos.
</commit_message>
<xml_diff>
--- a/bbdd/variables_alumnos_padres.xlsx
+++ b/bbdd/variables_alumnos_padres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josedanielconejeros/Dropbox/Fondecyt 2019-2021(AsistenteJC)/ciudadania-agencia/bbdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A844A393-5328-5342-98A0-C6E0283FF76A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D4E527-0824-ED40-9E36-1DDE6B6187E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
   </bookViews>
@@ -4381,11 +4381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4145EC5A-2CEF-EB47-8CDF-8C2465EE6ED9}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I256"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F265" sqref="F265"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4475,23 +4474,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>683</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>693</v>
-      </c>
-      <c r="E4" t="s">
-        <v>693</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>689</v>
       </c>
     </row>
@@ -4518,7 +4517,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>683</v>
       </c>
@@ -4538,7 +4537,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>683</v>
       </c>
@@ -4691,7 +4690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>683</v>
       </c>
@@ -4714,7 +4713,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>683</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>683</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>683</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>683</v>
       </c>
@@ -4806,7 +4805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>683</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>683</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>683</v>
       </c>
@@ -4875,7 +4874,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>683</v>
       </c>
@@ -4898,7 +4897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>683</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>683</v>
       </c>
@@ -4944,7 +4943,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>683</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>683</v>
       </c>
@@ -4990,7 +4989,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>683</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>683</v>
       </c>
@@ -5036,7 +5035,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>683</v>
       </c>
@@ -5059,7 +5058,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>683</v>
       </c>
@@ -5082,7 +5081,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>683</v>
       </c>
@@ -5105,7 +5104,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>683</v>
       </c>
@@ -5128,7 +5127,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>683</v>
       </c>
@@ -5154,7 +5153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>683</v>
       </c>
@@ -5180,7 +5179,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>683</v>
       </c>
@@ -5206,7 +5205,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>683</v>
       </c>
@@ -5232,7 +5231,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>683</v>
       </c>
@@ -5258,7 +5257,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>683</v>
       </c>
@@ -5284,7 +5283,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>683</v>
       </c>
@@ -5310,7 +5309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>683</v>
       </c>
@@ -5333,7 +5332,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>683</v>
       </c>
@@ -5356,7 +5355,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>683</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>683</v>
       </c>
@@ -5402,7 +5401,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>683</v>
       </c>
@@ -5425,7 +5424,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>683</v>
       </c>
@@ -6064,7 +6063,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>683</v>
       </c>
@@ -6113,7 +6112,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>683</v>
       </c>
@@ -6136,7 +6135,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>683</v>
       </c>
@@ -6159,7 +6158,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>683</v>
       </c>
@@ -6182,7 +6181,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>683</v>
       </c>
@@ -6205,7 +6204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>683</v>
       </c>
@@ -6228,7 +6227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>683</v>
       </c>
@@ -6251,7 +6250,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>683</v>
       </c>
@@ -6264,17 +6263,18 @@
       <c r="E76" t="s">
         <v>693</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>683</v>
       </c>
@@ -6287,17 +6287,18 @@
       <c r="E77" t="s">
         <v>693</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H77" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>683</v>
       </c>
@@ -6310,17 +6311,18 @@
       <c r="E78" t="s">
         <v>693</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H78" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>683</v>
       </c>
@@ -6333,17 +6335,18 @@
       <c r="E79" t="s">
         <v>693</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>683</v>
       </c>
@@ -6356,17 +6359,18 @@
       <c r="E80" t="s">
         <v>693</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>683</v>
       </c>
@@ -6379,17 +6383,18 @@
       <c r="E81" t="s">
         <v>693</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>683</v>
       </c>
@@ -6402,17 +6407,18 @@
       <c r="E82" t="s">
         <v>693</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H82" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>683</v>
       </c>
@@ -6435,7 +6441,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>683</v>
       </c>
@@ -6458,7 +6464,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>683</v>
       </c>
@@ -6481,7 +6487,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>683</v>
       </c>
@@ -6504,7 +6510,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>683</v>
       </c>
@@ -6527,7 +6533,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>683</v>
       </c>
@@ -6540,17 +6546,18 @@
       <c r="E88" t="s">
         <v>693</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H88" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>683</v>
       </c>
@@ -6563,17 +6570,18 @@
       <c r="E89" t="s">
         <v>693</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>683</v>
       </c>
@@ -6586,17 +6594,18 @@
       <c r="E90" t="s">
         <v>693</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>683</v>
       </c>
@@ -6609,17 +6618,18 @@
       <c r="E91" t="s">
         <v>693</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>683</v>
       </c>
@@ -6632,17 +6642,18 @@
       <c r="E92" t="s">
         <v>693</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H92" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>683</v>
       </c>
@@ -6655,17 +6666,18 @@
       <c r="E93" t="s">
         <v>693</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>683</v>
       </c>
@@ -6678,17 +6690,18 @@
       <c r="E94" t="s">
         <v>693</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H94" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>683</v>
       </c>
@@ -6711,7 +6724,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>683</v>
       </c>
@@ -6734,7 +6747,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>683</v>
       </c>
@@ -6757,7 +6770,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>683</v>
       </c>
@@ -6780,7 +6793,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>683</v>
       </c>
@@ -6803,7 +6816,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>683</v>
       </c>
@@ -6826,7 +6839,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>683</v>
       </c>
@@ -6849,7 +6862,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>683</v>
       </c>
@@ -6872,7 +6885,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>683</v>
       </c>
@@ -6895,7 +6908,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>683</v>
       </c>
@@ -6918,7 +6931,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>683</v>
       </c>
@@ -6941,7 +6954,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>683</v>
       </c>
@@ -6964,7 +6977,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>683</v>
       </c>
@@ -6987,7 +7000,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>683</v>
       </c>
@@ -7010,7 +7023,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>683</v>
       </c>
@@ -7033,7 +7046,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>683</v>
       </c>
@@ -7056,7 +7069,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>683</v>
       </c>
@@ -7079,7 +7092,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>683</v>
       </c>
@@ -7102,7 +7115,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>683</v>
       </c>
@@ -7125,7 +7138,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>683</v>
       </c>
@@ -7148,7 +7161,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>683</v>
       </c>
@@ -7171,7 +7184,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>683</v>
       </c>
@@ -7194,7 +7207,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>683</v>
       </c>
@@ -7217,7 +7230,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>683</v>
       </c>
@@ -7240,7 +7253,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>683</v>
       </c>
@@ -7263,7 +7276,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>683</v>
       </c>
@@ -7286,7 +7299,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>683</v>
       </c>
@@ -7309,7 +7322,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>683</v>
       </c>
@@ -7332,7 +7345,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>683</v>
       </c>
@@ -7875,7 +7888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>683</v>
       </c>
@@ -7898,7 +7911,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>683</v>
       </c>
@@ -7921,7 +7934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>683</v>
       </c>
@@ -7973,7 +7986,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>683</v>
       </c>
@@ -7996,7 +8009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>683</v>
       </c>
@@ -8019,7 +8032,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>683</v>
       </c>
@@ -8042,7 +8055,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>683</v>
       </c>
@@ -8065,7 +8078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>683</v>
       </c>
@@ -8088,7 +8101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>683</v>
       </c>
@@ -8345,7 +8358,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>683</v>
       </c>
@@ -8368,7 +8381,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>683</v>
       </c>
@@ -8391,7 +8404,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>683</v>
       </c>
@@ -8414,7 +8427,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>683</v>
       </c>
@@ -8437,7 +8450,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>683</v>
       </c>
@@ -8460,7 +8473,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>683</v>
       </c>
@@ -8483,7 +8496,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>683</v>
       </c>
@@ -8506,7 +8519,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>683</v>
       </c>
@@ -8529,7 +8542,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>683</v>
       </c>
@@ -8552,7 +8565,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>683</v>
       </c>
@@ -8575,7 +8588,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>683</v>
       </c>
@@ -8728,7 +8741,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>683</v>
       </c>
@@ -8751,7 +8764,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>683</v>
       </c>
@@ -8774,7 +8787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>683</v>
       </c>
@@ -8797,7 +8810,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>683</v>
       </c>
@@ -9938,7 +9951,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>614</v>
       </c>
@@ -9958,7 +9971,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>614</v>
       </c>
@@ -9978,7 +9991,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>614</v>
       </c>
@@ -9998,7 +10011,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>614</v>
       </c>
@@ -10021,7 +10034,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>614</v>
       </c>
@@ -10044,7 +10057,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>614</v>
       </c>
@@ -10070,7 +10083,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>614</v>
       </c>
@@ -10096,7 +10109,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>614</v>
       </c>
@@ -10122,7 +10135,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>614</v>
       </c>
@@ -10145,7 +10158,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>614</v>
       </c>
@@ -10168,7 +10181,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>614</v>
       </c>
@@ -10191,7 +10204,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>614</v>
       </c>
@@ -10214,7 +10227,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>614</v>
       </c>
@@ -10237,7 +10250,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>614</v>
       </c>
@@ -10260,7 +10273,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>614</v>
       </c>
@@ -10283,7 +10296,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>614</v>
       </c>
@@ -10306,7 +10319,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>614</v>
       </c>
@@ -10329,7 +10342,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>614</v>
       </c>
@@ -10352,7 +10365,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>614</v>
       </c>
@@ -10375,7 +10388,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>614</v>
       </c>
@@ -10398,7 +10411,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>614</v>
       </c>
@@ -10421,7 +10434,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>614</v>
       </c>
@@ -10444,7 +10457,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>614</v>
       </c>
@@ -10467,7 +10480,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>614</v>
       </c>
@@ -10490,7 +10503,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>614</v>
       </c>
@@ -10513,7 +10526,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>614</v>
       </c>
@@ -10536,7 +10549,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>614</v>
       </c>
@@ -10559,7 +10572,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>614</v>
       </c>
@@ -10582,7 +10595,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>614</v>
       </c>
@@ -10605,7 +10618,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>614</v>
       </c>
@@ -10628,7 +10641,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>614</v>
       </c>
@@ -10652,24 +10665,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I256" xr:uid="{087A14B9-0F2C-ED43-9E71-9CDDCDAB86A6}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Alumno y Padres"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I256" xr:uid="{087A14B9-0F2C-ED43-9E71-9CDDCDAB86A6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8A2E0A-F877-974D-8C0E-9CC503976022}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="D222" sqref="D222:D225"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10736,7 +10742,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>693</v>
       </c>
@@ -10773,7 +10779,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>693</v>
       </c>
@@ -10790,7 +10796,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>693</v>
       </c>
@@ -10907,7 +10913,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>693</v>
       </c>
@@ -10924,7 +10930,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>693</v>
       </c>
@@ -10941,7 +10947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>693</v>
       </c>
@@ -10958,7 +10964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>693</v>
       </c>
@@ -10975,7 +10981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>693</v>
       </c>
@@ -10992,7 +10998,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>693</v>
       </c>
@@ -11009,7 +11015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>693</v>
       </c>
@@ -11026,7 +11032,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>693</v>
       </c>
@@ -11043,7 +11049,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>693</v>
       </c>
@@ -11060,7 +11066,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>693</v>
       </c>
@@ -11077,7 +11083,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>693</v>
       </c>
@@ -11094,7 +11100,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>693</v>
       </c>
@@ -11111,7 +11117,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>693</v>
       </c>
@@ -11128,7 +11134,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>693</v>
       </c>
@@ -11145,7 +11151,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>693</v>
       </c>
@@ -11162,7 +11168,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>693</v>
       </c>
@@ -11179,7 +11185,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>693</v>
       </c>
@@ -11196,7 +11202,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>693</v>
       </c>
@@ -11213,7 +11219,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>693</v>
       </c>
@@ -11230,7 +11236,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>693</v>
       </c>
@@ -11247,7 +11253,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>693</v>
       </c>
@@ -11264,7 +11270,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>693</v>
       </c>
@@ -11281,7 +11287,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>693</v>
       </c>
@@ -11298,7 +11304,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>693</v>
       </c>
@@ -11315,7 +11321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>693</v>
       </c>
@@ -11332,7 +11338,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>693</v>
       </c>
@@ -11349,7 +11355,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>693</v>
       </c>
@@ -11366,7 +11372,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>693</v>
       </c>
@@ -11383,7 +11389,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>693</v>
       </c>
@@ -11400,7 +11406,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>693</v>
       </c>
@@ -11417,7 +11423,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>693</v>
       </c>
@@ -11434,7 +11440,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>693</v>
       </c>
@@ -11911,7 +11917,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>693</v>
       </c>
@@ -11948,7 +11954,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>693</v>
       </c>
@@ -11965,7 +11971,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>693</v>
       </c>
@@ -11982,7 +11988,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>693</v>
       </c>
@@ -11999,7 +12005,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>693</v>
       </c>
@@ -12016,7 +12022,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>693</v>
       </c>
@@ -12033,7 +12039,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>693</v>
       </c>
@@ -12050,7 +12056,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>693</v>
       </c>
@@ -12067,7 +12073,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>693</v>
       </c>
@@ -12084,7 +12090,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>693</v>
       </c>
@@ -12101,7 +12107,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>693</v>
       </c>
@@ -12118,7 +12124,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>693</v>
       </c>
@@ -12135,7 +12141,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>693</v>
       </c>
@@ -12152,7 +12158,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>693</v>
       </c>
@@ -12169,7 +12175,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>693</v>
       </c>
@@ -12186,7 +12192,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>693</v>
       </c>
@@ -12203,7 +12209,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>693</v>
       </c>
@@ -12220,7 +12226,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>693</v>
       </c>
@@ -12237,7 +12243,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>693</v>
       </c>
@@ -12254,7 +12260,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>693</v>
       </c>
@@ -12271,7 +12277,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>693</v>
       </c>
@@ -12288,7 +12294,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>693</v>
       </c>
@@ -12305,7 +12311,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>693</v>
       </c>
@@ -12322,7 +12328,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>693</v>
       </c>
@@ -12339,7 +12345,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>693</v>
       </c>
@@ -12356,7 +12362,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>693</v>
       </c>
@@ -12373,7 +12379,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>693</v>
       </c>
@@ -12390,7 +12396,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>693</v>
       </c>
@@ -12407,7 +12413,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>693</v>
       </c>
@@ -12424,7 +12430,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>693</v>
       </c>
@@ -12441,7 +12447,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>693</v>
       </c>
@@ -12458,7 +12464,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>693</v>
       </c>
@@ -12475,7 +12481,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>693</v>
       </c>
@@ -12492,7 +12498,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>693</v>
       </c>
@@ -12509,7 +12515,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>693</v>
       </c>
@@ -12526,7 +12532,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>693</v>
       </c>
@@ -12543,7 +12549,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>693</v>
       </c>
@@ -12560,7 +12566,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>693</v>
       </c>
@@ -12577,7 +12583,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>693</v>
       </c>
@@ -12594,7 +12600,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>693</v>
       </c>
@@ -12611,7 +12617,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>693</v>
       </c>
@@ -12628,7 +12634,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>693</v>
       </c>
@@ -12645,7 +12651,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>693</v>
       </c>
@@ -12662,7 +12668,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>693</v>
       </c>
@@ -12679,7 +12685,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>693</v>
       </c>
@@ -12696,7 +12702,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>693</v>
       </c>
@@ -12713,7 +12719,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>693</v>
       </c>
@@ -12730,7 +12736,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>693</v>
       </c>
@@ -12747,7 +12753,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>693</v>
       </c>
@@ -12764,7 +12770,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>693</v>
       </c>
@@ -12781,7 +12787,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>693</v>
       </c>
@@ -12798,7 +12804,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>693</v>
       </c>
@@ -12815,7 +12821,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>693</v>
       </c>
@@ -12832,7 +12838,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>693</v>
       </c>
@@ -12849,7 +12855,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>693</v>
       </c>
@@ -13266,7 +13272,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>693</v>
       </c>
@@ -13283,7 +13289,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>693</v>
       </c>
@@ -13300,7 +13306,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>693</v>
       </c>
@@ -13337,7 +13343,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>693</v>
       </c>
@@ -13354,7 +13360,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>693</v>
       </c>
@@ -13371,7 +13377,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>693</v>
       </c>
@@ -13388,7 +13394,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>693</v>
       </c>
@@ -13405,7 +13411,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>693</v>
       </c>
@@ -13422,7 +13428,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>693</v>
       </c>
@@ -13619,7 +13625,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>693</v>
       </c>
@@ -13636,7 +13642,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>693</v>
       </c>
@@ -13653,7 +13659,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>693</v>
       </c>
@@ -13670,7 +13676,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>693</v>
       </c>
@@ -13687,7 +13693,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>693</v>
       </c>
@@ -13704,7 +13710,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>693</v>
       </c>
@@ -13721,7 +13727,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>693</v>
       </c>
@@ -13738,7 +13744,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>693</v>
       </c>
@@ -13755,7 +13761,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>693</v>
       </c>
@@ -13772,7 +13778,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>693</v>
       </c>
@@ -13789,7 +13795,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>693</v>
       </c>
@@ -13906,7 +13912,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>693</v>
       </c>
@@ -13923,7 +13929,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>693</v>
       </c>
@@ -13940,7 +13946,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>693</v>
       </c>
@@ -13957,7 +13963,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>693</v>
       </c>
@@ -14834,7 +14840,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>614</v>
       </c>
@@ -14851,7 +14857,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>614</v>
       </c>
@@ -14868,7 +14874,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>614</v>
       </c>
@@ -14885,7 +14891,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>614</v>
       </c>
@@ -14902,7 +14908,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>614</v>
       </c>
@@ -14919,7 +14925,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>614</v>
       </c>
@@ -14936,7 +14942,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>614</v>
       </c>
@@ -14953,7 +14959,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>614</v>
       </c>
@@ -14970,7 +14976,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>614</v>
       </c>
@@ -14984,7 +14990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>614</v>
       </c>
@@ -14998,7 +15004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>614</v>
       </c>
@@ -15012,7 +15018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>614</v>
       </c>
@@ -15026,7 +15032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>614</v>
       </c>
@@ -15040,7 +15046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>614</v>
       </c>
@@ -15054,7 +15060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>614</v>
       </c>
@@ -15068,7 +15074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>614</v>
       </c>
@@ -15082,7 +15088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>614</v>
       </c>
@@ -15096,7 +15102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>614</v>
       </c>
@@ -15113,7 +15119,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>614</v>
       </c>
@@ -15130,7 +15136,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>614</v>
       </c>
@@ -15147,7 +15153,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>614</v>
       </c>
@@ -15164,7 +15170,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>614</v>
       </c>
@@ -15181,7 +15187,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>614</v>
       </c>
@@ -15198,7 +15204,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>614</v>
       </c>
@@ -15215,7 +15221,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>614</v>
       </c>
@@ -15232,7 +15238,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>614</v>
       </c>
@@ -15249,7 +15255,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>614</v>
       </c>
@@ -15266,7 +15272,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>614</v>
       </c>
@@ -15283,7 +15289,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>614</v>
       </c>
@@ -15300,7 +15306,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>614</v>
       </c>
@@ -15317,7 +15323,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>614</v>
       </c>
@@ -15335,13 +15341,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H256" xr:uid="{84E8F246-7C6E-DC47-A149-109CF80EF503}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Alumno y Padres"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H256" xr:uid="{84E8F246-7C6E-DC47-A149-109CF80EF503}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18334,7 +18334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F742D0C4-EA20-DA41-8D8B-CEEA081748BB}">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revisión de no respuesta en los cuestionarios
</commit_message>
<xml_diff>
--- a/bbdd/variables_alumnos_padres.xlsx
+++ b/bbdd/variables_alumnos_padres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josedanielconejeros/Dropbox/Fondecyt 2019-2021(AsistenteJC)/ciudadania-agencia/bbdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D4E527-0824-ED40-9E36-1DDE6B6187E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796C2062-7BEE-C545-B188-B3135514F221}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" activeTab="1" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" activeTab="4" xr2:uid="{66D1939E-F540-4C41-9398-9710D77FB3D3}"/>
   </bookViews>
   <sheets>
     <sheet name="alumnos_padres" sheetId="1" r:id="rId1"/>
@@ -10674,7 +10674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8A2E0A-F877-974D-8C0E-9CC503976022}">
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -20795,11 +20795,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFC846A-09B5-4C45-AF4B-7F6BDCC6C70A}">
   <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>